<commit_message>
add video analysis project add excel export to dir of test
</commit_message>
<xml_diff>
--- a/Xiaowen.Office.Excel/templates/account.xlsx
+++ b/Xiaowen.Office.Excel/templates/account.xlsx
@@ -24,11 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Account</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,13 +379,7 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>